<commit_message>
created corrrect three row output, need to put in csv
</commit_message>
<xml_diff>
--- a/Lab3/CityPop.xlsx
+++ b/Lab3/CityPop.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/labraham2_wisc_edu/Documents/School/Madison/courses/fall2017/GEOG 378/labs/Lab3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leanne\OneDrive for Business\OneDrive - UW-Madison\School\Madison\courses\fall2017\GEOG 378\labs\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="24CF87F1E760720957C566BB9B73397E7EE8B08D" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{51553EA7-3987-495D-A247-57AE2ECCE2B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CityPop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1053,14 +1054,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2982,6 +2992,24 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:N40">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="9" tint="-0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
it works! For real this time!
</commit_message>
<xml_diff>
--- a/Lab3/CityPop.xlsx
+++ b/Lab3/CityPop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leanne\OneDrive for Business\OneDrive - UW-Madison\School\Madison\courses\fall2017\GEOG 378\labs\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="24CF87F1E760720957C566BB9B73397E7EE8B08D" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{51553EA7-3987-495D-A247-57AE2ECCE2B6}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="24CF87F1E760720957C566BB9B73397E7EE8B08D" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{79C119DE-4095-452E-B5E1-2FCB3F14CC5F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CityPop" sheetId="1" r:id="rId1"/>
@@ -696,9 +696,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1057,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,7 +1070,7 @@
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1115,7 +1116,7 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1162,7 +1163,7 @@
       <c r="N2">
         <v>36.67</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <f>((N2-F2)/F2)</f>
         <v>0.57381974248927037</v>
       </c>
@@ -1210,7 +1211,7 @@
       <c r="N3">
         <v>22.16</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="2">
         <f t="shared" ref="O3:O40" si="0">((N3-F3)/F3)</f>
         <v>5.2776203966005664</v>
       </c>
@@ -1258,7 +1259,7 @@
       <c r="N4">
         <v>20.260000000000002</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>1.6587926509186353</v>
       </c>
@@ -1306,7 +1307,7 @@
       <c r="N5">
         <v>20.04</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="2">
         <f t="shared" si="0"/>
         <v>2.4492254733218592</v>
       </c>
@@ -1354,7 +1355,7 @@
       <c r="N6">
         <v>19.46</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="2">
         <f t="shared" si="0"/>
         <v>1.2189281641961234</v>
       </c>
@@ -1402,7 +1403,7 @@
       <c r="N7">
         <v>19.43</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="2">
         <f t="shared" si="0"/>
         <v>0.20012353304508945</v>
       </c>
@@ -1450,7 +1451,7 @@
       <c r="N8">
         <v>16.579999999999998</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="2">
         <f t="shared" si="0"/>
         <v>1.7450331125827814</v>
       </c>
@@ -1498,7 +1499,7 @@
       <c r="N9">
         <v>15.55</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="2">
         <f t="shared" si="0"/>
         <v>1.243867243867244</v>
       </c>
@@ -1546,7 +1547,7 @@
       <c r="N10">
         <v>14.65</v>
       </c>
-      <c r="O10" s="1" t="e">
+      <c r="O10" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="N11">
         <v>13.12</v>
       </c>
-      <c r="O11" s="1" t="e">
+      <c r="O11" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -1642,7 +1643,7 @@
       <c r="N12">
         <v>13.07</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="2">
         <f t="shared" si="0"/>
         <v>0.61358024691358037</v>
       </c>
@@ -1690,7 +1691,7 @@
       <c r="N13">
         <v>12.76</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="2">
         <f t="shared" si="0"/>
         <v>0.52267303102625284</v>
       </c>
@@ -1738,7 +1739,7 @@
       <c r="N14">
         <v>12.39</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="2">
         <f t="shared" si="0"/>
         <v>1.7968397291196392</v>
       </c>
@@ -1786,7 +1787,7 @@
       <c r="N15">
         <v>11.95</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="2">
         <f t="shared" si="0"/>
         <v>0.79969879518072284</v>
       </c>
@@ -1834,7 +1835,7 @@
       <c r="N16">
         <v>11.63</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="2">
         <f t="shared" si="0"/>
         <v>2.2946175637393771</v>
       </c>
@@ -1882,7 +1883,7 @@
       <c r="N17">
         <v>11.34</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="2">
         <f t="shared" si="0"/>
         <v>0.20510095642933046</v>
       </c>
@@ -1930,7 +1931,7 @@
       <c r="N18">
         <v>11</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="2">
         <f t="shared" si="0"/>
         <v>0.97132616487455192</v>
       </c>
@@ -1978,7 +1979,7 @@
       <c r="N19">
         <v>10.58</v>
       </c>
-      <c r="O19" s="1" t="e">
+      <c r="O19" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2026,7 +2027,7 @@
       <c r="N20">
         <v>10.55</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20" s="2">
         <f t="shared" si="0"/>
         <v>0.4838255977496484</v>
       </c>
@@ -2074,7 +2075,7 @@
       <c r="N21">
         <v>10.52</v>
       </c>
-      <c r="O21" s="1" t="e">
+      <c r="O21" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2122,7 +2123,7 @@
       <c r="N22">
         <v>10.49</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O22" s="2">
         <f t="shared" si="0"/>
         <v>0.25628742514970065</v>
       </c>
@@ -2170,7 +2171,7 @@
       <c r="N23">
         <v>9.77</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23" s="2">
         <f t="shared" si="0"/>
         <v>0.83992467043314512</v>
       </c>
@@ -2218,7 +2219,7 @@
       <c r="N24">
         <v>9.4</v>
       </c>
-      <c r="O24" s="1" t="e">
+      <c r="O24" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2266,7 +2267,7 @@
       <c r="N25">
         <v>9.2100000000000009</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O25" s="2">
         <f t="shared" si="0"/>
         <v>1.3494897959183676</v>
       </c>
@@ -2314,7 +2315,7 @@
       <c r="N26">
         <v>9.1999999999999993</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26" s="2">
         <f t="shared" si="0"/>
         <v>0.29395218002812923</v>
       </c>
@@ -2362,7 +2363,7 @@
       <c r="N27">
         <v>9.01</v>
       </c>
-      <c r="O27" s="1" t="e">
+      <c r="O27" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2410,7 +2411,7 @@
       <c r="N28">
         <v>8.94</v>
       </c>
-      <c r="O28" s="1" t="e">
+      <c r="O28" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2458,7 +2459,7 @@
       <c r="N29">
         <v>8.8800000000000008</v>
       </c>
-      <c r="O29" s="1" t="e">
+      <c r="O29" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2506,7 +2507,7 @@
       <c r="N30">
         <v>8.75</v>
       </c>
-      <c r="O30" s="1" t="e">
+      <c r="O30" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2554,7 +2555,7 @@
       <c r="N31">
         <v>8.6300000000000008</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O31" s="2">
         <f t="shared" si="0"/>
         <v>0.14913448735019988</v>
       </c>
@@ -2602,7 +2603,7 @@
       <c r="N32">
         <v>0</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2650,7 +2651,7 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O33" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2698,7 +2699,7 @@
       <c r="N34">
         <v>0</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O34" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2746,7 +2747,7 @@
       <c r="N35">
         <v>0</v>
       </c>
-      <c r="O35" s="1" t="e">
+      <c r="O35" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2794,7 +2795,7 @@
       <c r="N36">
         <v>0</v>
       </c>
-      <c r="O36" s="1" t="e">
+      <c r="O36" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2842,7 +2843,7 @@
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O37" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2890,7 +2891,7 @@
       <c r="N38">
         <v>0</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O38" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2938,7 +2939,7 @@
       <c r="N39">
         <v>0</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O39" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
@@ -2986,7 +2987,7 @@
       <c r="N40">
         <v>0</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O40" s="2">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>

</xml_diff>